<commit_message>
Ajustes de responsividade e implementações básicas
</commit_message>
<xml_diff>
--- a/resources/PROPOSTA  - COBERTURA PREMIUM.xlsx
+++ b/resources/PROPOSTA  - COBERTURA PREMIUM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Gabriela\pdf_generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF7E767-E25B-44BD-A07E-3FFB1C588DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2E2D32-472A-4F44-8212-94D2AAC72BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Nome:</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Data:</t>
-  </si>
-  <si>
-    <t>Data da Entrega:</t>
   </si>
   <si>
     <t>Valor:</t>
@@ -323,6 +320,12 @@
   <si>
     <t>[Valor p/ Forma de Pagamento]</t>
   </si>
+  <si>
+    <t>Prazo de Entrega:</t>
+  </si>
+  <si>
+    <t>40 dias úteis</t>
+  </si>
 </sst>
 </file>
 
@@ -1448,7 +1451,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="21" borderId="23" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="21" borderId="27" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="21" borderId="23" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="21" borderId="19" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="21" borderId="10" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1615,6 +1627,9 @@
     <xf numFmtId="0" fontId="38" fillId="21" borderId="11" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="23" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="21" borderId="23" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1636,15 +1651,6 @@
     <xf numFmtId="0" fontId="38" fillId="21" borderId="32" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="21" borderId="27" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="23" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="19" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="43" fillId="21" borderId="27" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1671,9 +1677,6 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="21" borderId="0" xfId="34" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="23" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="21" borderId="29" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2263,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="S43" sqref="S43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2309,18 +2312,18 @@
     </row>
     <row r="3" spans="2:16" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
       <c r="O3" s="19"/>
     </row>
     <row r="4" spans="2:16" ht="4.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2349,18 +2352,18 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="105" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="105"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="106"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="108"/>
+      <c r="L6" s="108"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="109"/>
       <c r="O6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="14.25" x14ac:dyDescent="0.2">
@@ -2370,15 +2373,15 @@
       <c r="E7" s="1"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="H7" s="103" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="103"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
-      <c r="N7" s="104"/>
+      <c r="H7" s="106" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="106"/>
+      <c r="M7" s="106"/>
+      <c r="N7" s="107"/>
       <c r="O7" s="28"/>
       <c r="P7" s="14"/>
     </row>
@@ -2389,15 +2392,15 @@
       <c r="E8" s="1"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
-      <c r="H8" s="103" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103"/>
-      <c r="N8" s="104"/>
+      <c r="H8" s="106" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="106"/>
+      <c r="J8" s="106"/>
+      <c r="K8" s="106"/>
+      <c r="L8" s="106"/>
+      <c r="M8" s="106"/>
+      <c r="N8" s="107"/>
       <c r="O8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2430,33 +2433,33 @@
       <c r="L10" s="33"/>
       <c r="M10" s="33"/>
       <c r="N10" s="34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O10" s="7"/>
     </row>
     <row r="11" spans="2:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="94" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
-      <c r="M11" s="94"/>
-      <c r="N11" s="95"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="97" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="97"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="97"/>
+      <c r="M11" s="97"/>
+      <c r="N11" s="98"/>
       <c r="O11" s="7"/>
     </row>
     <row r="12" spans="2:16" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -2470,20 +2473,20 @@
     </row>
     <row r="13" spans="2:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15"/>
-      <c r="C13" s="85" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="87"/>
+      <c r="C13" s="88" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="90"/>
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2492,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="66"/>
       <c r="F14" s="66"/>
@@ -2504,10 +2507,10 @@
         <v>9</v>
       </c>
       <c r="L14" s="65"/>
-      <c r="M14" s="96" t="s">
-        <v>32</v>
-      </c>
-      <c r="N14" s="97"/>
+      <c r="M14" s="99" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="100"/>
       <c r="O14" s="7"/>
     </row>
     <row r="15" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2516,7 +2519,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="68"/>
       <c r="F15" s="68"/>
@@ -2528,8 +2531,8 @@
       </c>
       <c r="K15" s="146"/>
       <c r="L15" s="146"/>
-      <c r="M15" s="144" t="s">
-        <v>33</v>
+      <c r="M15" s="69" t="s">
+        <v>32</v>
       </c>
       <c r="N15" s="145"/>
       <c r="O15" s="59"/>
@@ -2539,28 +2542,28 @@
       <c r="C16" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="82" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="83"/>
-      <c r="L16" s="83"/>
-      <c r="M16" s="83"/>
-      <c r="N16" s="84"/>
+      <c r="D16" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="86"/>
+      <c r="N16" s="87"/>
       <c r="O16" s="7"/>
     </row>
     <row r="17" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="28"/>
       <c r="C17" s="60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="69" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="69"/>
       <c r="F17" s="69"/>
@@ -2587,39 +2590,39 @@
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="90" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="91"/>
-      <c r="H19" s="91"/>
-      <c r="I19" s="91"/>
-      <c r="J19" s="91"/>
-      <c r="K19" s="91"/>
-      <c r="L19" s="92"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="94"/>
+      <c r="L19" s="95"/>
       <c r="M19" s="32" t="s">
         <v>8</v>
       </c>
       <c r="N19" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O19" s="7"/>
     </row>
     <row r="20" spans="2:15" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="14"/>
       <c r="C20" s="39"/>
-      <c r="D20" s="132"/>
-      <c r="E20" s="133"/>
-      <c r="F20" s="133"/>
-      <c r="G20" s="133"/>
-      <c r="H20" s="133"/>
-      <c r="I20" s="133"/>
-      <c r="J20" s="133"/>
-      <c r="K20" s="133"/>
-      <c r="L20" s="134"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="72"/>
       <c r="M20" s="37"/>
       <c r="N20" s="38"/>
       <c r="O20" s="7"/>
@@ -2627,15 +2630,15 @@
     <row r="21" spans="2:15" ht="52.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="14"/>
       <c r="C21" s="39"/>
-      <c r="D21" s="138"/>
-      <c r="E21" s="133"/>
-      <c r="F21" s="133"/>
-      <c r="G21" s="133"/>
-      <c r="H21" s="133"/>
-      <c r="I21" s="133"/>
-      <c r="J21" s="133"/>
-      <c r="K21" s="133"/>
-      <c r="L21" s="134"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="72"/>
       <c r="M21" s="37"/>
       <c r="N21" s="38"/>
       <c r="O21" s="7"/>
@@ -2963,15 +2966,15 @@
     <row r="42" spans="2:15" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="14"/>
       <c r="C42" s="16"/>
-      <c r="D42" s="111"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="112"/>
-      <c r="G42" s="112"/>
-      <c r="H42" s="112"/>
-      <c r="I42" s="112"/>
-      <c r="J42" s="112"/>
-      <c r="K42" s="112"/>
-      <c r="L42" s="113"/>
+      <c r="D42" s="114"/>
+      <c r="E42" s="115"/>
+      <c r="F42" s="115"/>
+      <c r="G42" s="115"/>
+      <c r="H42" s="115"/>
+      <c r="I42" s="115"/>
+      <c r="J42" s="115"/>
+      <c r="K42" s="115"/>
+      <c r="L42" s="116"/>
       <c r="M42" s="17"/>
       <c r="N42" s="18"/>
       <c r="O42" s="7"/>
@@ -2981,37 +2984,37 @@
       <c r="C43" s="16">
         <v>1</v>
       </c>
-      <c r="D43" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="76"/>
-      <c r="J43" s="76"/>
-      <c r="K43" s="76"/>
-      <c r="L43" s="77"/>
+      <c r="D43" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="79"/>
+      <c r="F43" s="79"/>
+      <c r="G43" s="79"/>
+      <c r="H43" s="79"/>
+      <c r="I43" s="79"/>
+      <c r="J43" s="79"/>
+      <c r="K43" s="79"/>
+      <c r="L43" s="80"/>
       <c r="M43" s="61" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N43" s="61" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="2:15" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="14"/>
       <c r="C44" s="16"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="118"/>
-      <c r="F44" s="118"/>
-      <c r="G44" s="118"/>
-      <c r="H44" s="118"/>
-      <c r="I44" s="118"/>
-      <c r="J44" s="118"/>
-      <c r="K44" s="118"/>
-      <c r="L44" s="119"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="121"/>
+      <c r="G44" s="121"/>
+      <c r="H44" s="121"/>
+      <c r="I44" s="121"/>
+      <c r="J44" s="121"/>
+      <c r="K44" s="121"/>
+      <c r="L44" s="122"/>
       <c r="M44" s="17"/>
       <c r="N44" s="18"/>
       <c r="O44" s="7"/>
@@ -3019,17 +3022,17 @@
     <row r="45" spans="2:15" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="14"/>
       <c r="C45" s="16"/>
-      <c r="D45" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="E45" s="73"/>
-      <c r="F45" s="73"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="73"/>
-      <c r="I45" s="73"/>
-      <c r="J45" s="73"/>
-      <c r="K45" s="73"/>
-      <c r="L45" s="74"/>
+      <c r="D45" s="75" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="76"/>
+      <c r="F45" s="76"/>
+      <c r="G45" s="76"/>
+      <c r="H45" s="76"/>
+      <c r="I45" s="76"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="77"/>
       <c r="M45" s="17"/>
       <c r="N45" s="18"/>
       <c r="O45" s="7"/>
@@ -3037,46 +3040,46 @@
     <row r="46" spans="2:15" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="14"/>
       <c r="C46" s="16"/>
-      <c r="D46" s="135" t="s">
-        <v>24</v>
-      </c>
-      <c r="E46" s="136"/>
-      <c r="F46" s="136"/>
-      <c r="G46" s="136"/>
-      <c r="H46" s="136"/>
-      <c r="I46" s="136"/>
-      <c r="J46" s="136"/>
-      <c r="K46" s="136"/>
-      <c r="L46" s="137"/>
+      <c r="D46" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="137"/>
+      <c r="F46" s="137"/>
+      <c r="G46" s="137"/>
+      <c r="H46" s="137"/>
+      <c r="I46" s="137"/>
+      <c r="J46" s="137"/>
+      <c r="K46" s="137"/>
+      <c r="L46" s="138"/>
       <c r="M46" s="17"/>
       <c r="N46" s="18"/>
       <c r="O46" s="7"/>
     </row>
     <row r="47" spans="2:15" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="14"/>
-      <c r="C47" s="98"/>
-      <c r="D47" s="99"/>
-      <c r="E47" s="99"/>
-      <c r="F47" s="99"/>
-      <c r="G47" s="99"/>
-      <c r="H47" s="99"/>
-      <c r="I47" s="100"/>
-      <c r="J47" s="109" t="s">
+      <c r="C47" s="101"/>
+      <c r="D47" s="102"/>
+      <c r="E47" s="102"/>
+      <c r="F47" s="102"/>
+      <c r="G47" s="102"/>
+      <c r="H47" s="102"/>
+      <c r="I47" s="103"/>
+      <c r="J47" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="K47" s="110"/>
-      <c r="L47" s="110"/>
-      <c r="M47" s="88" t="s">
-        <v>26</v>
-      </c>
-      <c r="N47" s="89"/>
+      <c r="K47" s="113"/>
+      <c r="L47" s="113"/>
+      <c r="M47" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="N47" s="92"/>
       <c r="O47" s="7"/>
     </row>
     <row r="48" spans="2:15" ht="1.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="14"/>
-      <c r="C48" s="93"/>
-      <c r="D48" s="93"/>
-      <c r="E48" s="93"/>
+      <c r="C48" s="96"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="96"/>
       <c r="F48" s="157"/>
       <c r="G48" s="157"/>
       <c r="H48" s="1"/>
@@ -3090,97 +3093,99 @@
     </row>
     <row r="49" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="14"/>
-      <c r="C49" s="79"/>
-      <c r="D49" s="80"/>
-      <c r="E49" s="80"/>
-      <c r="F49" s="80"/>
-      <c r="G49" s="80"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="80"/>
-      <c r="J49" s="80"/>
-      <c r="K49" s="80"/>
-      <c r="L49" s="80"/>
-      <c r="M49" s="80"/>
-      <c r="N49" s="81"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="83"/>
+      <c r="F49" s="83"/>
+      <c r="G49" s="83"/>
+      <c r="H49" s="83"/>
+      <c r="I49" s="83"/>
+      <c r="J49" s="83"/>
+      <c r="K49" s="83"/>
+      <c r="L49" s="83"/>
+      <c r="M49" s="83"/>
+      <c r="N49" s="84"/>
       <c r="O49" s="7"/>
     </row>
     <row r="50" spans="2:15" s="22" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="21"/>
-      <c r="C50" s="127" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="128"/>
+      <c r="C50" s="131" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="132"/>
       <c r="E50" s="40"/>
       <c r="F50" s="40"/>
       <c r="G50" s="40"/>
-      <c r="H50" s="125"/>
-      <c r="I50" s="125"/>
-      <c r="J50" s="125"/>
-      <c r="K50" s="125"/>
-      <c r="L50" s="125"/>
-      <c r="M50" s="125"/>
-      <c r="N50" s="126"/>
+      <c r="H50" s="128" t="s">
+        <v>35</v>
+      </c>
+      <c r="I50" s="129"/>
+      <c r="J50" s="129"/>
+      <c r="K50" s="129"/>
+      <c r="L50" s="129"/>
+      <c r="M50" s="129"/>
+      <c r="N50" s="130"/>
       <c r="O50" s="7"/>
     </row>
     <row r="51" spans="2:15" s="22" customFormat="1" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="21"/>
-      <c r="C51" s="122"/>
-      <c r="D51" s="123"/>
-      <c r="E51" s="123"/>
-      <c r="F51" s="123"/>
-      <c r="G51" s="123"/>
-      <c r="H51" s="123"/>
-      <c r="I51" s="123"/>
-      <c r="J51" s="123"/>
-      <c r="K51" s="123"/>
-      <c r="L51" s="123"/>
-      <c r="M51" s="123"/>
-      <c r="N51" s="124"/>
+      <c r="C51" s="125"/>
+      <c r="D51" s="126"/>
+      <c r="E51" s="126"/>
+      <c r="F51" s="126"/>
+      <c r="G51" s="126"/>
+      <c r="H51" s="126"/>
+      <c r="I51" s="126"/>
+      <c r="J51" s="126"/>
+      <c r="K51" s="126"/>
+      <c r="L51" s="126"/>
+      <c r="M51" s="126"/>
+      <c r="N51" s="127"/>
       <c r="O51" s="7"/>
     </row>
     <row r="52" spans="2:15" s="22" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="21"/>
-      <c r="C52" s="142" t="s">
+      <c r="C52" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="D52" s="143"/>
-      <c r="E52" s="130"/>
-      <c r="F52" s="130"/>
+      <c r="D52" s="144"/>
+      <c r="E52" s="134"/>
+      <c r="F52" s="134"/>
       <c r="G52" s="41"/>
-      <c r="H52" s="140" t="s">
-        <v>34</v>
-      </c>
-      <c r="I52" s="140"/>
-      <c r="J52" s="140"/>
-      <c r="K52" s="140"/>
-      <c r="L52" s="140"/>
-      <c r="M52" s="140"/>
-      <c r="N52" s="141"/>
+      <c r="H52" s="141" t="s">
+        <v>33</v>
+      </c>
+      <c r="I52" s="141"/>
+      <c r="J52" s="141"/>
+      <c r="K52" s="141"/>
+      <c r="L52" s="141"/>
+      <c r="M52" s="141"/>
+      <c r="N52" s="142"/>
       <c r="O52" s="7"/>
     </row>
     <row r="53" spans="2:15" s="22" customFormat="1" ht="21" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="21"/>
-      <c r="C53" s="129"/>
+      <c r="C53" s="133"/>
       <c r="D53" s="42"/>
       <c r="E53" s="43"/>
       <c r="F53" s="43"/>
       <c r="G53" s="43"/>
-      <c r="H53" s="116"/>
+      <c r="H53" s="119"/>
       <c r="I53" s="154"/>
-      <c r="J53" s="139"/>
-      <c r="K53" s="139"/>
-      <c r="L53" s="139"/>
-      <c r="M53" s="116"/>
-      <c r="N53" s="117"/>
+      <c r="J53" s="140"/>
+      <c r="K53" s="140"/>
+      <c r="L53" s="140"/>
+      <c r="M53" s="119"/>
+      <c r="N53" s="120"/>
       <c r="O53" s="7"/>
     </row>
     <row r="54" spans="2:15" s="22" customFormat="1" ht="21" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="21"/>
-      <c r="C54" s="129"/>
+      <c r="C54" s="133"/>
       <c r="D54" s="44"/>
       <c r="E54" s="45"/>
       <c r="F54" s="46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G54" s="152"/>
       <c r="H54" s="152"/>
@@ -3194,20 +3199,20 @@
     </row>
     <row r="55" spans="2:15" s="22" customFormat="1" ht="27.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="21"/>
-      <c r="C55" s="129"/>
+      <c r="C55" s="133"/>
       <c r="D55" s="47"/>
       <c r="E55" s="48"/>
       <c r="F55" s="49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G55" s="50"/>
-      <c r="H55" s="120"/>
+      <c r="H55" s="123"/>
       <c r="I55" s="156"/>
       <c r="J55" s="151"/>
       <c r="K55" s="151"/>
       <c r="L55" s="151"/>
-      <c r="M55" s="120"/>
-      <c r="N55" s="121"/>
+      <c r="M55" s="123"/>
+      <c r="N55" s="124"/>
       <c r="O55" s="7"/>
     </row>
     <row r="56" spans="2:15" s="22" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3218,36 +3223,36 @@
       <c r="F56" s="52"/>
       <c r="G56" s="52"/>
       <c r="H56" s="52"/>
-      <c r="I56" s="114"/>
-      <c r="J56" s="114"/>
-      <c r="K56" s="114"/>
-      <c r="L56" s="114"/>
-      <c r="M56" s="114"/>
-      <c r="N56" s="115"/>
+      <c r="I56" s="117"/>
+      <c r="J56" s="117"/>
+      <c r="K56" s="117"/>
+      <c r="L56" s="117"/>
+      <c r="M56" s="117"/>
+      <c r="N56" s="118"/>
       <c r="O56" s="7"/>
     </row>
     <row r="57" spans="2:15" s="22" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="21"/>
-      <c r="C57" s="107" t="s">
-        <v>22</v>
-      </c>
-      <c r="D57" s="108"/>
-      <c r="E57" s="108"/>
-      <c r="F57" s="108"/>
-      <c r="G57" s="108"/>
+      <c r="C57" s="110" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="111"/>
+      <c r="E57" s="111"/>
+      <c r="F57" s="111"/>
+      <c r="G57" s="111"/>
       <c r="H57" s="53"/>
       <c r="I57" s="54"/>
-      <c r="J57" s="108"/>
-      <c r="K57" s="108"/>
-      <c r="L57" s="108"/>
-      <c r="M57" s="108"/>
-      <c r="N57" s="131"/>
+      <c r="J57" s="111"/>
+      <c r="K57" s="111"/>
+      <c r="L57" s="111"/>
+      <c r="M57" s="111"/>
+      <c r="N57" s="135"/>
       <c r="O57" s="7"/>
     </row>
     <row r="58" spans="2:15" s="22" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="21"/>
       <c r="C58" s="55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D58" s="56"/>
       <c r="E58" s="56"/>
@@ -3313,6 +3318,7 @@
     <mergeCell ref="D36:L36"/>
     <mergeCell ref="D37:L37"/>
     <mergeCell ref="D30:L30"/>
+    <mergeCell ref="D27:L27"/>
     <mergeCell ref="H6:N6"/>
     <mergeCell ref="H7:N7"/>
     <mergeCell ref="C57:G57"/>
@@ -3345,7 +3351,6 @@
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="D22:L22"/>
     <mergeCell ref="H8:N8"/>
-    <mergeCell ref="D27:L27"/>
     <mergeCell ref="D25:L25"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="D14:J14"/>

</xml_diff>